<commit_message>
updating listener and extent reports
</commit_message>
<xml_diff>
--- a/src/test/java/com/tutorials/ninja/qa/testdata/tutorialsNinjaValidCredentials.xlsx
+++ b/src/test/java/com/tutorials/ninja/qa/testdata/tutorialsNinjaValidCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafia Sultana\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792CEC70-6D59-4E74-AE79-7637C59E44CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34790AA0-9099-4686-BD35-3C07EF0026E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4F758E6E-2CFA-4726-A442-E7A90296F81F}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>rafiasultana12345@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Selenium@123</t>
   </si>
@@ -50,32 +47,23 @@
     <t>Password</t>
   </si>
   <si>
-    <t>rafiasultana122@yahoo.com</t>
-  </si>
-  <si>
-    <t>ss123456@gmail.com</t>
-  </si>
-  <si>
-    <t>sharmin@123</t>
-  </si>
-  <si>
-    <t>rashidmohammed@yahoo.com</t>
-  </si>
-  <si>
-    <t>mohammed@123</t>
-  </si>
-  <si>
-    <t>akhterrashida@gmail.com</t>
-  </si>
-  <si>
-    <t>rashida@123</t>
+    <t>rafselenium1@gmail.com</t>
+  </si>
+  <si>
+    <t>rafselenium2@gmail.com</t>
+  </si>
+  <si>
+    <t>rafselenium3@yahoo.com</t>
+  </si>
+  <si>
+    <t>rafselenium4@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +75,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,11 +128,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7C89-9DD6-4E7C-BF22-3AFCEE842A1D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,18 +463,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -487,34 +482,51 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{59CABDBC-5A23-4BA4-85A6-EF36064EA5E4}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{3F19AC36-C416-46A7-A922-1E7E04C6AA67}"/>
@@ -523,7 +535,7 @@
     <hyperlink ref="B4" r:id="rId5" xr:uid="{14328E6B-4D46-47BA-A916-6AE17EEB5BD9}"/>
     <hyperlink ref="A5" r:id="rId6" xr:uid="{CE7EE16A-FCC7-40AD-A238-BF35A7C26B8F}"/>
     <hyperlink ref="B5" r:id="rId7" xr:uid="{C383738D-8A47-46B8-97A2-EC4DFFC0B658}"/>
-    <hyperlink ref="B6" r:id="rId8" xr:uid="{B6BA8179-AB05-4F61-9BA3-4A2E7D8B808E}"/>
+    <hyperlink ref="A4" r:id="rId8" xr:uid="{6725289E-DA5A-4695-B1E9-D89097F9BAB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>